<commit_message>
20240401 Update to Cloud
</commit_message>
<xml_diff>
--- a/data/load_solar_profile/Load_02.xlsx
+++ b/data/load_solar_profile/Load_02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Operation Data\Moaz Afzal\Daily &amp; Monthly Reports\Monthly Reports\Generation and Distribution Record\GEN and Dis Data\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevWork\EEM-2\EEM-2\data\load_solar_profile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD57189E-C8F2-4A17-B875-C2CA5432EDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884EA869-69A1-4490-AC4D-F0850A4A2A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19785" windowHeight="11760" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Summary Min,Max,AVG" sheetId="33" r:id="rId1"/>
@@ -48,6 +48,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1321,14 +1332,23 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1348,23 +1368,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="6" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1406,9 +1417,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1446,7 +1457,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1552,7 +1563,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1694,7 +1705,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1705,7 +1716,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1780,7 +1791,7 @@
       </c>
       <c r="D5" s="72">
         <f>'Indvidual Summary'!G34</f>
-        <v>1355.4862637362637</v>
+        <v>1351.8010204081631</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2256,24 +2267,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5073,24 +5084,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7894,24 +7905,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10711,24 +10722,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13530,24 +13541,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16350,24 +16361,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19169,24 +19180,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21986,24 +21997,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24805,24 +24816,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27622,24 +27633,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30436,100 +30447,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:83" s="29" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
-      <c r="AB1" s="124"/>
-      <c r="AC1" s="124"/>
-      <c r="AD1" s="124"/>
-      <c r="AE1" s="124"/>
-      <c r="AF1" s="124"/>
-      <c r="AG1" s="124"/>
-      <c r="AH1" s="124"/>
-      <c r="AI1" s="124"/>
-      <c r="AJ1" s="124"/>
-      <c r="AK1" s="124"/>
-      <c r="AL1" s="124"/>
-      <c r="AM1" s="124"/>
-      <c r="AN1" s="124"/>
-      <c r="AO1" s="124"/>
-      <c r="AP1" s="124"/>
-      <c r="AQ1" s="124"/>
-      <c r="AR1" s="124"/>
-      <c r="AS1" s="124"/>
-      <c r="AT1" s="124"/>
-      <c r="AU1" s="124"/>
-      <c r="AV1" s="124"/>
-      <c r="AW1" s="124"/>
-      <c r="AX1" s="124"/>
-      <c r="AY1" s="124"/>
-      <c r="AZ1" s="124"/>
-      <c r="BA1" s="124"/>
-      <c r="BB1" s="124"/>
-      <c r="BC1" s="124"/>
-      <c r="BD1" s="124"/>
-      <c r="BE1" s="124"/>
-      <c r="BF1" s="124"/>
-      <c r="BG1" s="124"/>
-      <c r="BH1" s="124"/>
-      <c r="BI1" s="124"/>
-      <c r="BJ1" s="124"/>
-      <c r="BK1" s="124"/>
-      <c r="BL1" s="124"/>
-      <c r="BM1" s="124"/>
-      <c r="BN1" s="124"/>
-      <c r="BO1" s="124"/>
-      <c r="BP1" s="124"/>
-      <c r="BQ1" s="124"/>
-      <c r="BR1" s="124"/>
-      <c r="BS1" s="124"/>
-      <c r="BT1" s="124"/>
-      <c r="BU1" s="124"/>
-      <c r="BV1" s="124"/>
-      <c r="BW1" s="124"/>
-      <c r="BX1" s="124"/>
-      <c r="BY1" s="124"/>
-      <c r="BZ1" s="124"/>
-      <c r="CA1" s="124"/>
-      <c r="CB1" s="125"/>
-      <c r="CC1" s="125"/>
-      <c r="CD1" s="126"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
+      <c r="AB1" s="115"/>
+      <c r="AC1" s="115"/>
+      <c r="AD1" s="115"/>
+      <c r="AE1" s="115"/>
+      <c r="AF1" s="115"/>
+      <c r="AG1" s="115"/>
+      <c r="AH1" s="115"/>
+      <c r="AI1" s="115"/>
+      <c r="AJ1" s="115"/>
+      <c r="AK1" s="115"/>
+      <c r="AL1" s="115"/>
+      <c r="AM1" s="115"/>
+      <c r="AN1" s="115"/>
+      <c r="AO1" s="115"/>
+      <c r="AP1" s="115"/>
+      <c r="AQ1" s="115"/>
+      <c r="AR1" s="115"/>
+      <c r="AS1" s="115"/>
+      <c r="AT1" s="115"/>
+      <c r="AU1" s="115"/>
+      <c r="AV1" s="115"/>
+      <c r="AW1" s="115"/>
+      <c r="AX1" s="115"/>
+      <c r="AY1" s="115"/>
+      <c r="AZ1" s="115"/>
+      <c r="BA1" s="115"/>
+      <c r="BB1" s="115"/>
+      <c r="BC1" s="115"/>
+      <c r="BD1" s="115"/>
+      <c r="BE1" s="115"/>
+      <c r="BF1" s="115"/>
+      <c r="BG1" s="115"/>
+      <c r="BH1" s="115"/>
+      <c r="BI1" s="115"/>
+      <c r="BJ1" s="115"/>
+      <c r="BK1" s="115"/>
+      <c r="BL1" s="115"/>
+      <c r="BM1" s="115"/>
+      <c r="BN1" s="115"/>
+      <c r="BO1" s="115"/>
+      <c r="BP1" s="115"/>
+      <c r="BQ1" s="115"/>
+      <c r="BR1" s="115"/>
+      <c r="BS1" s="115"/>
+      <c r="BT1" s="115"/>
+      <c r="BU1" s="115"/>
+      <c r="BV1" s="115"/>
+      <c r="BW1" s="115"/>
+      <c r="BX1" s="115"/>
+      <c r="BY1" s="115"/>
+      <c r="BZ1" s="115"/>
+      <c r="CA1" s="115"/>
+      <c r="CB1" s="116"/>
+      <c r="CC1" s="116"/>
+      <c r="CD1" s="117"/>
     </row>
     <row r="2" spans="1:83" s="31" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="114"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
       <c r="E2" s="109" t="s">
         <v>2</v>
       </c>
@@ -30580,90 +30591,90 @@
       </c>
       <c r="AG2" s="110"/>
       <c r="AH2" s="111"/>
-      <c r="AI2" s="115" t="s">
+      <c r="AI2" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="116"/>
-      <c r="AK2" s="117"/>
-      <c r="AL2" s="115" t="s">
+      <c r="AJ2" s="119"/>
+      <c r="AK2" s="120"/>
+      <c r="AL2" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="AM2" s="116"/>
-      <c r="AN2" s="117"/>
-      <c r="AO2" s="115" t="s">
+      <c r="AM2" s="119"/>
+      <c r="AN2" s="120"/>
+      <c r="AO2" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="AP2" s="116"/>
-      <c r="AQ2" s="117"/>
-      <c r="AR2" s="115" t="s">
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="120"/>
+      <c r="AR2" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="AS2" s="116"/>
-      <c r="AT2" s="117"/>
-      <c r="AU2" s="115" t="s">
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="120"/>
+      <c r="AU2" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="AV2" s="116"/>
-      <c r="AW2" s="117"/>
-      <c r="AX2" s="115" t="s">
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="120"/>
+      <c r="AX2" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="AY2" s="116"/>
-      <c r="AZ2" s="117"/>
-      <c r="BA2" s="115" t="s">
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="120"/>
+      <c r="BA2" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="BB2" s="116"/>
-      <c r="BC2" s="117"/>
-      <c r="BD2" s="115" t="s">
+      <c r="BB2" s="119"/>
+      <c r="BC2" s="120"/>
+      <c r="BD2" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="BE2" s="116"/>
-      <c r="BF2" s="117"/>
-      <c r="BG2" s="115" t="s">
+      <c r="BE2" s="119"/>
+      <c r="BF2" s="120"/>
+      <c r="BG2" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="BH2" s="116"/>
-      <c r="BI2" s="117"/>
-      <c r="BJ2" s="115" t="s">
+      <c r="BH2" s="119"/>
+      <c r="BI2" s="120"/>
+      <c r="BJ2" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="BK2" s="116"/>
-      <c r="BL2" s="117"/>
-      <c r="BM2" s="115" t="s">
+      <c r="BK2" s="119"/>
+      <c r="BL2" s="120"/>
+      <c r="BM2" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="BN2" s="116"/>
-      <c r="BO2" s="117"/>
-      <c r="BP2" s="115" t="s">
+      <c r="BN2" s="119"/>
+      <c r="BO2" s="120"/>
+      <c r="BP2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="BQ2" s="116"/>
-      <c r="BR2" s="117"/>
-      <c r="BS2" s="115" t="s">
+      <c r="BQ2" s="119"/>
+      <c r="BR2" s="120"/>
+      <c r="BS2" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="BT2" s="116"/>
-      <c r="BU2" s="117"/>
-      <c r="BV2" s="115" t="s">
+      <c r="BT2" s="119"/>
+      <c r="BU2" s="120"/>
+      <c r="BV2" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="BW2" s="116"/>
-      <c r="BX2" s="117"/>
-      <c r="BY2" s="115" t="s">
+      <c r="BW2" s="119"/>
+      <c r="BX2" s="120"/>
+      <c r="BY2" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="BZ2" s="116"/>
-      <c r="CA2" s="116"/>
-      <c r="CB2" s="118" t="s">
+      <c r="BZ2" s="119"/>
+      <c r="CA2" s="119"/>
+      <c r="CB2" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="CC2" s="119"/>
-      <c r="CD2" s="120"/>
+      <c r="CC2" s="122"/>
+      <c r="CD2" s="123"/>
       <c r="CE2" s="30"/>
     </row>
     <row r="3" spans="1:83" s="38" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="122"/>
+      <c r="A3" s="113"/>
       <c r="B3" s="46" t="s">
         <v>18</v>
       </c>
@@ -38193,7 +38204,7 @@
       </c>
       <c r="G26" s="19">
         <f>'23'!C29</f>
-        <v>1444.6153846153845</v>
+        <v>1341.4285714285713</v>
       </c>
       <c r="H26" s="78">
         <f>'23'!D27</f>
@@ -40408,7 +40419,7 @@
         <v>0</v>
       </c>
       <c r="BN32" s="39">
-        <f t="shared" ref="BN32:CS32" si="2">MIN(BN4:BN31)</f>
+        <f t="shared" ref="BN32:CD32" si="2">MIN(BN4:BN31)</f>
         <v>20</v>
       </c>
       <c r="BO32" s="39">
@@ -40833,7 +40844,7 @@
       </c>
       <c r="G34" s="21">
         <f t="shared" si="6"/>
-        <v>1355.4862637362637</v>
+        <v>1351.8010204081631</v>
       </c>
       <c r="H34" s="24">
         <f t="shared" si="6"/>
@@ -41794,6 +41805,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="CB2:CD2"/>
+    <mergeCell ref="BY2:CA2"/>
+    <mergeCell ref="BV2:BX2"/>
+    <mergeCell ref="BS2:BU2"/>
+    <mergeCell ref="BP2:BR2"/>
+    <mergeCell ref="BM2:BO2"/>
     <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="T2:V2"/>
@@ -41810,19 +41834,6 @@
     <mergeCell ref="BD2:BF2"/>
     <mergeCell ref="BA2:BC2"/>
     <mergeCell ref="AX2:AZ2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="CB2:CD2"/>
-    <mergeCell ref="BY2:CA2"/>
-    <mergeCell ref="BV2:BX2"/>
-    <mergeCell ref="BS2:BU2"/>
-    <mergeCell ref="BP2:BR2"/>
-    <mergeCell ref="BM2:BO2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="11" orientation="landscape" r:id="rId1"/>
@@ -41864,24 +41875,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -44683,24 +44694,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -47502,24 +47513,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -50321,24 +50332,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -53141,24 +53152,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -55928,8 +55939,8 @@
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="39" zoomScaleNormal="39" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="39" zoomScaleNormal="39" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55964,24 +55975,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -57575,7 +57586,9 @@
         <f t="shared" si="0"/>
         <v>4303</v>
       </c>
-      <c r="C20" s="89"/>
+      <c r="C20" s="89">
+        <v>0</v>
+      </c>
       <c r="D20" s="89">
         <v>1080</v>
       </c>
@@ -58419,7 +58432,7 @@
       </c>
       <c r="C29" s="20">
         <f>AVERAGE(C9:C22)</f>
-        <v>1444.6153846153845</v>
+        <v>1341.4285714285713</v>
       </c>
       <c r="D29" s="20">
         <f t="shared" ref="D29:AB29" si="3">AVERAGE(D3:D26)</f>
@@ -58781,24 +58794,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -61602,24 +61615,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -64419,24 +64432,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -67236,24 +67249,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -70056,24 +70069,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -72873,24 +72886,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -75692,24 +75705,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -78508,24 +78521,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -81325,24 +81338,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -84142,24 +84155,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -86964,24 +86977,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -89784,24 +89797,24 @@
       <c r="I1" s="130"/>
       <c r="J1" s="130"/>
       <c r="K1" s="131"/>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
       <c r="AB1" s="132"/>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>